<commit_message>
1. move talking step table to single file 2. record item to excel one by one
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>鞋子</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +53,14 @@
   </si>
   <si>
     <t>官银</t>
+  </si>
+  <si>
+    <t>台子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>银子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -404,7 +412,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -455,6 +463,19 @@
         <v>30.5</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="E8">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>7.5</v>
+      </c>
+    </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="G12" t="s">
         <v>9</v>
@@ -468,6 +489,14 @@
         <v>10</v>
       </c>
       <c r="H13">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14">
         <v>7.8</v>
       </c>
     </row>

</xml_diff>